<commit_message>
calculated releant quantities (tissue fraction area, length of centerlines, width (tissue fraction area/length), and total area of the image) of entropy-filtered images belonging to day 1 and day 7 for slides 25-27 and 10-11. Radius of structuring element is 34 pixels corresponding to 5 um.
</commit_message>
<xml_diff>
--- a/Image_Analysis/tissue_image_data.xlsx
+++ b/Image_Analysis/tissue_image_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tfai/Documents/GitHub/Minimal-Lung-Model/Image_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DAFE22-AB3B-C649-A797-FB58EC472B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E063E385-31D5-E747-B49E-FA0178184AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380"/>
   </bookViews>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="true" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -446,7 +446,8 @@
     <col min="5" max="5" width="3.5703125" customWidth="true"/>
     <col min="7" max="7" width="7.140625" customWidth="true"/>
     <col min="8" max="8" width="9.28515625" customWidth="true"/>
-    <col min="9" max="9" width="13.7109375" customWidth="true"/>
+    <col min="9" max="9" width="14.7109375" customWidth="true"/>
+    <col min="11" max="11" width="9.1640625" bestFit="true" customWidth="true"/>
     <col min="6" max="6" width="3.5703125" customWidth="true"/>
   </cols>
   <sheetData>
@@ -1332,294 +1333,1657 @@
         <v>1.4527969888265994E-2</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="0">
-        <v>1</v>
-      </c>
-      <c r="B31" s="0">
+    <row r="31" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
         <v>26</v>
       </c>
-      <c r="C31" s="0">
-        <v>1</v>
-      </c>
-      <c r="D31" s="0">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
         <v>0.18633587170605814</v>
       </c>
-      <c r="E31" s="0">
-        <v>19</v>
-      </c>
-      <c r="F31" s="0">
-        <v>19</v>
-      </c>
-      <c r="G31" s="0">
+      <c r="E31">
+        <v>19</v>
+      </c>
+      <c r="F31">
+        <v>19</v>
+      </c>
+      <c r="G31">
         <v>50330</v>
       </c>
-      <c r="H31" s="0">
+      <c r="H31">
         <v>2985047</v>
       </c>
-      <c r="I31" s="0">
-        <v>0.016860706045834454</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="0">
-        <v>1</v>
-      </c>
-      <c r="B32" s="0">
+      <c r="I31">
+        <v>1.6860706045834454E-2</v>
+      </c>
+    </row>
+    <row r="32" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
         <v>26</v>
       </c>
-      <c r="C32" s="0">
+      <c r="C32">
         <v>2</v>
       </c>
-      <c r="D32" s="0">
+      <c r="D32">
         <v>0.21482258857088068</v>
       </c>
-      <c r="E32" s="0">
-        <v>19</v>
-      </c>
-      <c r="F32" s="0">
-        <v>19</v>
-      </c>
-      <c r="G32" s="0">
+      <c r="E32">
+        <v>19</v>
+      </c>
+      <c r="F32">
+        <v>19</v>
+      </c>
+      <c r="G32">
         <v>61734</v>
       </c>
-      <c r="H32" s="0">
+      <c r="H32">
         <v>3441396</v>
       </c>
-      <c r="I32" s="0">
-        <v>0.017938650477887463</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="0">
-        <v>1</v>
-      </c>
-      <c r="B33" s="0">
+      <c r="I32">
+        <v>1.7938650477887463E-2</v>
+      </c>
+    </row>
+    <row r="33" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
         <v>26</v>
       </c>
-      <c r="C33" s="0">
+      <c r="C33">
         <v>3</v>
       </c>
-      <c r="D33" s="0">
+      <c r="D33">
         <v>0.225996384953737</v>
       </c>
-      <c r="E33" s="0">
-        <v>19</v>
-      </c>
-      <c r="F33" s="0">
-        <v>19</v>
-      </c>
-      <c r="G33" s="0">
+      <c r="E33">
+        <v>19</v>
+      </c>
+      <c r="F33">
+        <v>19</v>
+      </c>
+      <c r="G33">
         <v>60728</v>
       </c>
-      <c r="H33" s="0">
+      <c r="H33">
         <v>3620397</v>
       </c>
-      <c r="I33" s="0">
-        <v>0.016773851044512521</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="0">
-        <v>1</v>
-      </c>
-      <c r="B34" s="0">
+      <c r="I33">
+        <v>1.6773851044512521E-2</v>
+      </c>
+    </row>
+    <row r="34" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
         <v>26</v>
       </c>
-      <c r="C34" s="0">
+      <c r="C34">
         <v>4</v>
       </c>
-      <c r="D34" s="0">
+      <c r="D34">
         <v>0.23650568749300863</v>
       </c>
-      <c r="E34" s="0">
-        <v>19</v>
-      </c>
-      <c r="F34" s="0">
-        <v>19</v>
-      </c>
-      <c r="G34" s="0">
+      <c r="E34">
+        <v>19</v>
+      </c>
+      <c r="F34">
+        <v>19</v>
+      </c>
+      <c r="G34">
         <v>61119</v>
       </c>
-      <c r="H34" s="0">
+      <c r="H34">
         <v>3788753</v>
       </c>
-      <c r="I34" s="0">
-        <v>0.016131692934324302</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="0">
-        <v>1</v>
-      </c>
-      <c r="B35" s="0">
+      <c r="I34">
+        <v>1.6131692934324302E-2</v>
+      </c>
+    </row>
+    <row r="35" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
         <v>26</v>
       </c>
-      <c r="C35" s="0">
+      <c r="C35">
         <v>5</v>
       </c>
-      <c r="D35" s="0">
+      <c r="D35">
         <v>0.22585237487415505</v>
       </c>
-      <c r="E35" s="0">
-        <v>19</v>
-      </c>
-      <c r="F35" s="0">
-        <v>19</v>
-      </c>
-      <c r="G35" s="0">
+      <c r="E35">
+        <v>19</v>
+      </c>
+      <c r="F35">
+        <v>19</v>
+      </c>
+      <c r="G35">
         <v>58502</v>
       </c>
-      <c r="H35" s="0">
+      <c r="H35">
         <v>3618090</v>
       </c>
-      <c r="I35" s="0">
-        <v>0.016169304798940878</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="0">
-        <v>1</v>
-      </c>
-      <c r="B36" s="0">
+      <c r="I35">
+        <v>1.6169304798940878E-2</v>
+      </c>
+    </row>
+    <row r="36" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
         <v>26</v>
       </c>
-      <c r="C36" s="0">
+      <c r="C36">
         <v>6</v>
       </c>
-      <c r="D36" s="0">
+      <c r="D36">
         <v>0.24341723496652123</v>
       </c>
-      <c r="E36" s="0">
-        <v>19</v>
-      </c>
-      <c r="F36" s="0">
-        <v>19</v>
-      </c>
-      <c r="G36" s="0">
+      <c r="E36">
+        <v>19</v>
+      </c>
+      <c r="F36">
+        <v>19</v>
+      </c>
+      <c r="G36">
         <v>66694</v>
       </c>
-      <c r="H36" s="0">
+      <c r="H36">
         <v>3899474</v>
       </c>
-      <c r="I36" s="0">
-        <v>0.017103332398164469</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="0">
-        <v>1</v>
-      </c>
-      <c r="B37" s="0">
+      <c r="I36">
+        <v>1.7103332398164469E-2</v>
+      </c>
+    </row>
+    <row r="37" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
         <v>26</v>
       </c>
-      <c r="C37" s="0">
-        <v>7</v>
-      </c>
-      <c r="D37" s="0">
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37">
         <v>0.24415488867714974</v>
       </c>
-      <c r="E37" s="0">
-        <v>19</v>
-      </c>
-      <c r="F37" s="0">
-        <v>19</v>
-      </c>
-      <c r="G37" s="0">
+      <c r="E37">
+        <v>19</v>
+      </c>
+      <c r="F37">
+        <v>19</v>
+      </c>
+      <c r="G37">
         <v>67779</v>
       </c>
-      <c r="H37" s="0">
+      <c r="H37">
         <v>3911291</v>
       </c>
-      <c r="I37" s="0">
-        <v>0.017329060916203884</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="0">
-        <v>1</v>
-      </c>
-      <c r="B38" s="0">
+      <c r="I37">
+        <v>1.7329060916203884E-2</v>
+      </c>
+    </row>
+    <row r="38" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
         <v>26</v>
       </c>
-      <c r="C38" s="0">
+      <c r="C38">
         <v>8</v>
       </c>
-      <c r="D38" s="0">
+      <c r="D38">
         <v>0.21468138753056235</v>
       </c>
-      <c r="E38" s="0">
-        <v>19</v>
-      </c>
-      <c r="F38" s="0">
-        <v>19</v>
-      </c>
-      <c r="G38" s="0">
+      <c r="E38">
+        <v>19</v>
+      </c>
+      <c r="F38">
+        <v>19</v>
+      </c>
+      <c r="G38">
         <v>60451</v>
       </c>
-      <c r="H38" s="0">
+      <c r="H38">
         <v>3439134</v>
       </c>
-      <c r="I38" s="0">
-        <v>0.017577390122048168</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="0">
-        <v>1</v>
-      </c>
-      <c r="B39" s="0">
+      <c r="I38">
+        <v>1.7577390122048168E-2</v>
+      </c>
+    </row>
+    <row r="39" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
         <v>26</v>
       </c>
-      <c r="C39" s="0">
+      <c r="C39">
         <v>9</v>
       </c>
-      <c r="D39" s="0">
+      <c r="D39">
         <v>0.21823369858334532</v>
       </c>
-      <c r="E39" s="0">
-        <v>19</v>
-      </c>
-      <c r="F39" s="0">
-        <v>19</v>
-      </c>
-      <c r="G39" s="0">
+      <c r="E39">
+        <v>19</v>
+      </c>
+      <c r="F39">
+        <v>19</v>
+      </c>
+      <c r="G39">
         <v>56825</v>
       </c>
-      <c r="H39" s="0">
+      <c r="H39">
         <v>3496041</v>
       </c>
-      <c r="I39" s="0">
-        <v>0.016254099994822715</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="0">
-        <v>1</v>
-      </c>
-      <c r="B40" s="0">
+      <c r="I39">
+        <v>1.6254099994822715E-2</v>
+      </c>
+    </row>
+    <row r="40" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="B40">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0.35518197830273102</v>
+      </c>
+      <c r="E40">
+        <v>19</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>62506</v>
+      </c>
+      <c r="H40">
+        <v>5689913</v>
+      </c>
+      <c r="I40">
+        <v>1.0985405225000805E-2</v>
+      </c>
+    </row>
+    <row r="41" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>0.35688987417501639</v>
+      </c>
+      <c r="E41">
+        <v>19</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>65337</v>
+      </c>
+      <c r="H41">
+        <v>5717273</v>
+      </c>
+      <c r="I41">
+        <v>1.1428000726919985E-2</v>
+      </c>
+    </row>
+    <row r="42" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>0.42149659119964206</v>
+      </c>
+      <c r="E42">
+        <v>19</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>77178</v>
+      </c>
+      <c r="H42">
+        <v>6752254</v>
+      </c>
+      <c r="I42">
+        <v>1.1429961017461725E-2</v>
+      </c>
+    </row>
+    <row r="43" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>0.36609590734215447</v>
+      </c>
+      <c r="E43">
+        <v>19</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>66648</v>
+      </c>
+      <c r="H43">
+        <v>5864751</v>
+      </c>
+      <c r="I43">
+        <v>1.1364165332850448E-2</v>
+      </c>
+    </row>
+    <row r="44" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44">
+        <v>0.40625823984850662</v>
+      </c>
+      <c r="E44">
+        <v>19</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>73168</v>
+      </c>
+      <c r="H44">
+        <v>6508140</v>
+      </c>
+      <c r="I44">
+        <v>1.124253626996346E-2</v>
+      </c>
+    </row>
+    <row r="45" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>7</v>
+      </c>
+      <c r="B45">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45">
+        <v>0.36715972172283745</v>
+      </c>
+      <c r="E45">
+        <v>19</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>65768</v>
+      </c>
+      <c r="H45">
+        <v>5881793</v>
+      </c>
+      <c r="I45">
+        <v>1.118162437882462E-2</v>
+      </c>
+    </row>
+    <row r="46" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>11</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>0.36726453009891813</v>
+      </c>
+      <c r="E46">
+        <v>19</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>63266</v>
+      </c>
+      <c r="H46">
+        <v>5883472</v>
+      </c>
+      <c r="I46">
+        <v>1.0753174316118101E-2</v>
+      </c>
+    </row>
+    <row r="47" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>11</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>0.39524574474247726</v>
+      </c>
+      <c r="E47">
+        <v>19</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>72810</v>
+      </c>
+      <c r="H47">
+        <v>6331723</v>
+      </c>
+      <c r="I47">
+        <v>1.1499239622453477E-2</v>
+      </c>
+    </row>
+    <row r="48" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>7</v>
+      </c>
+      <c r="B48">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>9</v>
+      </c>
+      <c r="D48">
+        <v>0.36482697067213193</v>
+      </c>
+      <c r="E48">
+        <v>19</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>65809</v>
+      </c>
+      <c r="H48">
+        <v>5844423</v>
+      </c>
+      <c r="I48">
+        <v>1.1260136372743725E-2</v>
+      </c>
+    </row>
+    <row r="49" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>7</v>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0.48832063897278555</v>
+      </c>
+      <c r="E49">
+        <v>34</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>65890</v>
+      </c>
+      <c r="H49">
+        <v>7822756</v>
+      </c>
+      <c r="I49">
+        <v>8.4228627353326625E-3</v>
+      </c>
+    </row>
+    <row r="50" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>7</v>
+      </c>
+      <c r="B50">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>0.48857726031529158</v>
+      </c>
+      <c r="E50">
+        <v>34</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>63677</v>
+      </c>
+      <c r="H50">
+        <v>7826867</v>
+      </c>
+      <c r="I50">
+        <v>8.1356946527901906E-3</v>
+      </c>
+    </row>
+    <row r="51" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>7</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>0.44714717717771707</v>
+      </c>
+      <c r="E51">
+        <v>34</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>53361</v>
+      </c>
+      <c r="H51">
+        <v>7163169</v>
+      </c>
+      <c r="I51">
+        <v>7.4493565627168643E-3</v>
+      </c>
+    </row>
+    <row r="52" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>7</v>
+      </c>
+      <c r="B52">
+        <v>10</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>0.52122903333093629</v>
+      </c>
+      <c r="E52">
+        <v>34</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>65891</v>
+      </c>
+      <c r="H52">
+        <v>8349939</v>
+      </c>
+      <c r="I52">
+        <v>7.89119537280452E-3</v>
+      </c>
+    </row>
+    <row r="53" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>7</v>
+      </c>
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>0.51325080001438228</v>
+      </c>
+      <c r="E53">
+        <v>34</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>69675</v>
+      </c>
+      <c r="H53">
+        <v>8222130</v>
+      </c>
+      <c r="I53">
+        <v>8.4740815336172021E-3</v>
+      </c>
+    </row>
+    <row r="54" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>7</v>
+      </c>
+      <c r="B54">
+        <v>10</v>
+      </c>
+      <c r="C54">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <v>0.48548007604631094</v>
+      </c>
+      <c r="E54">
+        <v>34</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>68870</v>
+      </c>
+      <c r="H54">
+        <v>7777251</v>
+      </c>
+      <c r="I54">
+        <v>8.8553140434840024E-3</v>
+      </c>
+    </row>
+    <row r="55" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>7</v>
+      </c>
+      <c r="B55">
+        <v>10</v>
+      </c>
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>0.54773100789826934</v>
+      </c>
+      <c r="E55">
+        <v>34</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>70035</v>
+      </c>
+      <c r="H55">
+        <v>8774493</v>
+      </c>
+      <c r="I55">
+        <v>7.9816577436439915E-3</v>
+      </c>
+    </row>
+    <row r="56" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>7</v>
+      </c>
+      <c r="B56">
+        <v>10</v>
+      </c>
+      <c r="C56">
+        <v>8</v>
+      </c>
+      <c r="D56">
+        <v>0.5247239775596465</v>
+      </c>
+      <c r="E56">
+        <v>34</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>72125</v>
+      </c>
+      <c r="H56">
+        <v>8405927</v>
+      </c>
+      <c r="I56">
+        <v>8.5802553365024459E-3</v>
+      </c>
+    </row>
+    <row r="57" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>7</v>
+      </c>
+      <c r="B57">
+        <v>10</v>
+      </c>
+      <c r="C57">
+        <v>9</v>
+      </c>
+      <c r="D57">
+        <v>0.51200327446585803</v>
+      </c>
+      <c r="E57">
+        <v>34</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>65219</v>
+      </c>
+      <c r="H57">
+        <v>8202145</v>
+      </c>
+      <c r="I57">
+        <v>7.951456600681894E-3</v>
+      </c>
+    </row>
+    <row r="58" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>7</v>
+      </c>
+      <c r="B58">
+        <v>10</v>
+      </c>
+      <c r="C58">
+        <v>10</v>
+      </c>
+      <c r="D58">
+        <v>0.45997206441663868</v>
+      </c>
+      <c r="E58">
+        <v>34</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>54717</v>
+      </c>
+      <c r="H58">
+        <v>7368620</v>
+      </c>
+      <c r="I58">
+        <v>7.4256780781204621E-3</v>
+      </c>
+    </row>
+    <row r="59" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>7</v>
+      </c>
+      <c r="B59">
+        <v>10</v>
+      </c>
+      <c r="C59">
+        <v>11</v>
+      </c>
+      <c r="D59">
+        <v>0.50375300130239542</v>
+      </c>
+      <c r="E59">
+        <v>34</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>63858</v>
+      </c>
+      <c r="H59">
+        <v>8069978</v>
+      </c>
+      <c r="I59">
+        <v>7.9130327245006127E-3</v>
+      </c>
+    </row>
+    <row r="60" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>25</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>0.42371710552599195</v>
+      </c>
+      <c r="E60">
+        <v>34</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>47970</v>
+      </c>
+      <c r="H60">
+        <v>6787826</v>
+      </c>
+      <c r="I60">
+        <v>7.0670638876129113E-3</v>
+      </c>
+    </row>
+    <row r="61" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>25</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>0.39332124073141889</v>
+      </c>
+      <c r="E61">
+        <v>34</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>45056</v>
+      </c>
+      <c r="H61">
+        <v>6300893</v>
+      </c>
+      <c r="I61">
+        <v>7.150732443798046E-3</v>
+      </c>
+    </row>
+    <row r="62" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>25</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>0.37033830570736853</v>
+      </c>
+      <c r="E62">
+        <v>34</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>43962</v>
+      </c>
+      <c r="H62">
+        <v>5932713</v>
+      </c>
+      <c r="I62">
+        <v>7.4101005728745015E-3</v>
+      </c>
+    </row>
+    <row r="63" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>25</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63">
+        <v>0.42505714210093165</v>
+      </c>
+      <c r="E63">
+        <v>34</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>44843</v>
+      </c>
+      <c r="H63">
+        <v>6809293</v>
+      </c>
+      <c r="I63">
+        <v>6.5855588825447812E-3</v>
+      </c>
+    </row>
+    <row r="64" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>25</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <v>0.40336861236956068</v>
+      </c>
+      <c r="E64">
+        <v>34</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>42739</v>
+      </c>
+      <c r="H64">
+        <v>6461849</v>
+      </c>
+      <c r="I64">
+        <v>6.6140511794689104E-3</v>
+      </c>
+    </row>
+    <row r="65" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>25</v>
+      </c>
+      <c r="C65">
+        <v>6</v>
+      </c>
+      <c r="D65">
+        <v>0.37741664769004585</v>
+      </c>
+      <c r="E65">
+        <v>34</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>44218</v>
+      </c>
+      <c r="H65">
+        <v>6046106</v>
+      </c>
+      <c r="I65">
+        <v>7.3134675442342563E-3</v>
+      </c>
+    </row>
+    <row r="66" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>25</v>
+      </c>
+      <c r="C66">
+        <v>7</v>
+      </c>
+      <c r="D66">
+        <v>0.38257572920162358</v>
+      </c>
+      <c r="E66">
+        <v>34</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>44272</v>
+      </c>
+      <c r="H66">
+        <v>6128753</v>
+      </c>
+      <c r="I66">
+        <v>7.2236554483432434E-3</v>
+      </c>
+    </row>
+    <row r="67" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>25</v>
+      </c>
+      <c r="C67">
+        <v>8</v>
+      </c>
+      <c r="D67">
+        <v>0.40279163570481169</v>
+      </c>
+      <c r="E67">
+        <v>34</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>46936</v>
+      </c>
+      <c r="H67">
+        <v>6452606</v>
+      </c>
+      <c r="I67">
+        <v>7.273960319288052E-3</v>
+      </c>
+    </row>
+    <row r="68" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>25</v>
+      </c>
+      <c r="C68">
+        <v>9</v>
+      </c>
+      <c r="D68">
+        <v>0.41184741648289308</v>
+      </c>
+      <c r="E68">
+        <v>34</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>46336</v>
+      </c>
+      <c r="H68">
+        <v>6597677</v>
+      </c>
+      <c r="I68">
+        <v>7.0230779712313895E-3</v>
+      </c>
+    </row>
+    <row r="69" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69">
         <v>26</v>
       </c>
-      <c r="C40" s="0">
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>0.33173037068331818</v>
+      </c>
+      <c r="E69">
+        <v>34</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>43837</v>
+      </c>
+      <c r="H69">
+        <v>5314225</v>
+      </c>
+      <c r="I69">
+        <v>8.2489920919795456E-3</v>
+      </c>
+    </row>
+    <row r="70" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>26</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>0.38444230458075651</v>
+      </c>
+      <c r="E70">
+        <v>34</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>53752</v>
+      </c>
+      <c r="H70">
+        <v>6158655</v>
+      </c>
+      <c r="I70">
+        <v>8.727879707501069E-3</v>
+      </c>
+    </row>
+    <row r="71" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>26</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>0.39497701331959029</v>
+      </c>
+      <c r="E71">
+        <v>34</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>51384</v>
+      </c>
+      <c r="H71">
+        <v>6327418</v>
+      </c>
+      <c r="I71">
+        <v>8.120848029954714E-3</v>
+      </c>
+    </row>
+    <row r="72" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>26</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <v>0.39624376518129667</v>
+      </c>
+      <c r="E72">
+        <v>34</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>50254</v>
+      </c>
+      <c r="H72">
+        <v>6347711</v>
+      </c>
+      <c r="I72">
+        <v>7.9168695613269103E-3</v>
+      </c>
+    </row>
+    <row r="73" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>26</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>0.3815489941392205</v>
+      </c>
+      <c r="E73">
+        <v>34</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>49571</v>
+      </c>
+      <c r="H73">
+        <v>6112305</v>
+      </c>
+      <c r="I73">
+        <v>8.1100337761286449E-3</v>
+      </c>
+    </row>
+    <row r="74" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>26</v>
+      </c>
+      <c r="C74">
+        <v>6</v>
+      </c>
+      <c r="D74">
+        <v>0.41231284307732874</v>
+      </c>
+      <c r="E74">
+        <v>34</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>52995</v>
+      </c>
+      <c r="H74">
+        <v>6605133</v>
+      </c>
+      <c r="I74">
+        <v>8.0233055110321017E-3</v>
+      </c>
+    </row>
+    <row r="75" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>26</v>
+      </c>
+      <c r="C75">
+        <v>7</v>
+      </c>
+      <c r="D75">
+        <v>0.41782267995829137</v>
+      </c>
+      <c r="E75">
+        <v>34</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>55330</v>
+      </c>
+      <c r="H75">
+        <v>6693399</v>
+      </c>
+      <c r="I75">
+        <v>8.266353163766272E-3</v>
+      </c>
+    </row>
+    <row r="76" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>26</v>
+      </c>
+      <c r="C76">
+        <v>8</v>
+      </c>
+      <c r="D76">
+        <v>0.38518039525304826</v>
+      </c>
+      <c r="E76">
+        <v>34</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>52430</v>
+      </c>
+      <c r="H76">
+        <v>6170479</v>
+      </c>
+      <c r="I76">
+        <v>8.4969092350853145E-3</v>
+      </c>
+    </row>
+    <row r="77" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77">
+        <v>26</v>
+      </c>
+      <c r="C77">
+        <v>9</v>
+      </c>
+      <c r="D77">
+        <v>0.37843376959585789</v>
+      </c>
+      <c r="E77">
+        <v>34</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>47585</v>
+      </c>
+      <c r="H77">
+        <v>6062400</v>
+      </c>
+      <c r="I77">
+        <v>7.8492016363156513E-3</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="0">
+        <v>1</v>
+      </c>
+      <c r="B78" s="0">
+        <v>27</v>
+      </c>
+      <c r="C78" s="0">
+        <v>1</v>
+      </c>
+      <c r="D78" s="0">
+        <v>0.51110800244099275</v>
+      </c>
+      <c r="E78" s="0">
+        <v>34</v>
+      </c>
+      <c r="F78" s="0">
+        <v>0</v>
+      </c>
+      <c r="G78" s="0">
+        <v>58407</v>
+      </c>
+      <c r="H78" s="0">
+        <v>8187803</v>
+      </c>
+      <c r="I78" s="0">
+        <v>0.0071334153984896802</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="0">
+        <v>1</v>
+      </c>
+      <c r="B79" s="0">
+        <v>27</v>
+      </c>
+      <c r="C79" s="0">
+        <v>2</v>
+      </c>
+      <c r="D79" s="0">
+        <v>0.50151463397094775</v>
+      </c>
+      <c r="E79" s="0">
+        <v>34</v>
+      </c>
+      <c r="F79" s="0">
+        <v>0</v>
+      </c>
+      <c r="G79" s="0">
+        <v>55170</v>
+      </c>
+      <c r="H79" s="0">
+        <v>8034120</v>
+      </c>
+      <c r="I79" s="0">
+        <v>0.0068669624053412197</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0">
+        <v>1</v>
+      </c>
+      <c r="B80" s="0">
+        <v>27</v>
+      </c>
+      <c r="C80" s="0">
+        <v>3</v>
+      </c>
+      <c r="D80" s="0">
+        <v>0.50242857050114265</v>
+      </c>
+      <c r="E80" s="0">
+        <v>34</v>
+      </c>
+      <c r="F80" s="0">
+        <v>0</v>
+      </c>
+      <c r="G80" s="0">
+        <v>53873</v>
+      </c>
+      <c r="H80" s="0">
+        <v>8048761</v>
+      </c>
+      <c r="I80" s="0">
+        <v>0.0066933283271797981</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0">
+        <v>1</v>
+      </c>
+      <c r="B81" s="0">
+        <v>27</v>
+      </c>
+      <c r="C81" s="0">
+        <v>4</v>
+      </c>
+      <c r="D81" s="0">
+        <v>0.51807273439123003</v>
+      </c>
+      <c r="E81" s="0">
+        <v>34</v>
+      </c>
+      <c r="F81" s="0">
+        <v>0</v>
+      </c>
+      <c r="G81" s="0">
+        <v>57493</v>
+      </c>
+      <c r="H81" s="0">
+        <v>8299376</v>
+      </c>
+      <c r="I81" s="0">
+        <v>0.0069273882759378538</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="0">
+        <v>1</v>
+      </c>
+      <c r="B82" s="0">
+        <v>27</v>
+      </c>
+      <c r="C82" s="0">
+        <v>5</v>
+      </c>
+      <c r="D82" s="0">
+        <v>0.56778779793294665</v>
+      </c>
+      <c r="E82" s="0">
+        <v>34</v>
+      </c>
+      <c r="F82" s="0">
+        <v>0</v>
+      </c>
+      <c r="G82" s="0">
+        <v>65056</v>
+      </c>
+      <c r="H82" s="0">
+        <v>9095797</v>
+      </c>
+      <c r="I82" s="0">
+        <v>0.0071523144151084284</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="0">
+        <v>1</v>
+      </c>
+      <c r="B83" s="0">
+        <v>27</v>
+      </c>
+      <c r="C83" s="0">
+        <v>6</v>
+      </c>
+      <c r="D83" s="0">
+        <v>0.44775330542771308</v>
+      </c>
+      <c r="E83" s="0">
+        <v>34</v>
+      </c>
+      <c r="F83" s="0">
+        <v>0</v>
+      </c>
+      <c r="G83" s="0">
+        <v>52776</v>
+      </c>
+      <c r="H83" s="0">
+        <v>7172879</v>
+      </c>
+      <c r="I83" s="0">
+        <v>0.0073577150820472509</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="0">
+        <v>1</v>
+      </c>
+      <c r="B84" s="0">
+        <v>27</v>
+      </c>
+      <c r="C84" s="0">
+        <v>7</v>
+      </c>
+      <c r="D84" s="0">
+        <v>0.6288651131805616</v>
+      </c>
+      <c r="E84" s="0">
+        <v>34</v>
+      </c>
+      <c r="F84" s="0">
+        <v>0</v>
+      </c>
+      <c r="G84" s="0">
+        <v>72308</v>
+      </c>
+      <c r="H84" s="0">
+        <v>10074238</v>
+      </c>
+      <c r="I84" s="0">
+        <v>0.007177515559985778</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0">
+        <v>1</v>
+      </c>
+      <c r="B85" s="0">
+        <v>27</v>
+      </c>
+      <c r="C85" s="0">
+        <v>8</v>
+      </c>
+      <c r="D85" s="0">
+        <v>0.52252949366380619</v>
+      </c>
+      <c r="E85" s="0">
+        <v>34</v>
+      </c>
+      <c r="F85" s="0">
+        <v>0</v>
+      </c>
+      <c r="G85" s="0">
+        <v>52304</v>
+      </c>
+      <c r="H85" s="0">
+        <v>8370772</v>
+      </c>
+      <c r="I85" s="0">
+        <v>0.006248408151601788</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0">
+        <v>1</v>
+      </c>
+      <c r="B86" s="0">
+        <v>27</v>
+      </c>
+      <c r="C86" s="0">
+        <v>9</v>
+      </c>
+      <c r="D86" s="0">
+        <v>0.52777234696853481</v>
+      </c>
+      <c r="E86" s="0">
+        <v>34</v>
+      </c>
+      <c r="F86" s="0">
+        <v>0</v>
+      </c>
+      <c r="G86" s="0">
+        <v>54247</v>
+      </c>
+      <c r="H86" s="0">
+        <v>8454761</v>
+      </c>
+      <c r="I86" s="0">
+        <v>0.0064161482506720179</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0">
+        <v>1</v>
+      </c>
+      <c r="B87" s="0">
+        <v>27</v>
+      </c>
+      <c r="C87" s="0">
         <v>10</v>
       </c>
-      <c r="D40" s="0">
-        <v>0.20605226860507855</v>
-      </c>
-      <c r="E40" s="0">
-        <v>19</v>
-      </c>
-      <c r="F40" s="0">
-        <v>19</v>
-      </c>
-      <c r="G40" s="0">
-        <v>51899</v>
-      </c>
-      <c r="H40" s="0">
-        <v>3300898</v>
-      </c>
-      <c r="I40" s="0">
-        <v>0.015722691219177326</v>
+      <c r="D87" s="0">
+        <v>0.51841281541141315</v>
+      </c>
+      <c r="E87" s="0">
+        <v>34</v>
+      </c>
+      <c r="F87" s="0">
+        <v>0</v>
+      </c>
+      <c r="G87" s="0">
+        <v>57839</v>
+      </c>
+      <c r="H87" s="0">
+        <v>8304824</v>
+      </c>
+      <c r="I87" s="0">
+        <v>0.0069645064121768262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made a complete table of all data
wrote the R code to merge all 3 tables
</commit_message>
<xml_diff>
--- a/Image_Analysis/tissue_image_data.xlsx
+++ b/Image_Analysis/tissue_image_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tfai/Documents/GitHub/Minimal-Lung-Model/Image_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C1C421-787D-9242-909E-2544B81A75C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7C66F0-547D-204E-8F0F-A02A92097E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1198,9 +1198,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z288"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A280" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H295" sqref="H295"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6884,7 +6884,7 @@
         <v>120.48106060606061</v>
       </c>
       <c r="J151">
-        <f t="shared" ref="J151:J182" si="2">1/I151</f>
+        <f t="shared" ref="J151:J172" si="2">1/I151</f>
         <v>8.3000597352783975E-3</v>
       </c>
       <c r="K151" s="65">
@@ -11560,8 +11560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E74E1D8-73D4-144E-9DC4-801AA327A535}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>